<commit_message>
Importaciones programacion maquinas y plan ciclos maquina
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Maquinas.xlsx
+++ b/planning/assets/formatsXlsx/Maquinas.xlsx
@@ -72,7 +72,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -80,6 +80,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <bottom style="thin">
@@ -102,60 +163,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -173,7 +180,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:A6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="0" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:A6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <tableColumns count="1">
     <tableColumn id="1" name="maquina" dataDxfId="1"/>
   </tableColumns>
@@ -469,7 +476,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>